<commit_message>
add 5/16 stuff to reports
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-16.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-16.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Train Runs" sheetId="1" r:id="rId1"/>
@@ -2415,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q127" sqref="Q127"/>
+    <sheetView showGridLines="0" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R146" sqref="R146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14509,8 +14509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:K21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15456,7 +15456,7 @@
         <v>CANFIELD</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>424</v>
+        <v>96</v>
       </c>
       <c r="N22" s="21" t="s">
         <v>504</v>
@@ -15501,7 +15501,7 @@
         <v>GOODNIGHT</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>424</v>
+        <v>96</v>
       </c>
       <c r="N23" s="21" t="s">
         <v>502</v>
@@ -15546,7 +15546,7 @@
         <v>GOODNIGHT</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>424</v>
+        <v>96</v>
       </c>
       <c r="N24" s="21" t="s">
         <v>503</v>
@@ -16804,7 +16804,7 @@
       <c r="L55" s="53"/>
       <c r="M55" s="17">
         <f>COUNTIF(M3:M52,"=Y")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16823,7 +16823,7 @@
       <c r="L56" s="54"/>
       <c r="M56" s="15">
         <f>COUNTA(M3:M52)-M55</f>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>